<commit_message>
Update components, CANService, Interface and Unit Tests, Add optional Failure Message Sent
</commit_message>
<xml_diff>
--- a/resources/Pinbelegung.xlsx
+++ b/resources/Pinbelegung.xlsx
@@ -1,17 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HofSpannung\Git\CarSoftware CAN Service\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA37BD3-BEF8-4A94-809A-DD0381ECC59F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="150" windowWidth="23715" windowHeight="4950"/>
+    <workbookView xWindow="240" yWindow="150" windowWidth="23715" windowHeight="4950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -150,8 +164,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,8 +173,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,6 +205,16 @@
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -207,10 +245,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
@@ -232,8 +272,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Gut" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -242,14 +286,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -287,9 +334,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -322,9 +369,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -357,9 +421,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -532,11 +613,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +655,7 @@
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="C6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
@@ -582,7 +663,7 @@
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
+      <c r="C7" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
@@ -590,7 +671,7 @@
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="C8" s="9" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
@@ -601,7 +682,7 @@
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
+      <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
@@ -610,7 +691,7 @@
       <c r="E9" s="6"/>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="C10" s="9" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
@@ -674,7 +755,7 @@
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="C19" s="10" t="s">
         <v>13</v>
       </c>
       <c r="D19" t="s">
@@ -683,7 +764,7 @@
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+      <c r="C20" s="10" t="s">
         <v>14</v>
       </c>
       <c r="D20" t="s">
@@ -692,7 +773,7 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+      <c r="C21" s="10" t="s">
         <v>15</v>
       </c>
       <c r="D21" t="s">
@@ -719,7 +800,7 @@
       </c>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+      <c r="C26" s="9" t="s">
         <v>33</v>
       </c>
       <c r="D26" t="s">
@@ -789,7 +870,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -801,7 +882,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Add RPM Sensor Message Handler
</commit_message>
<xml_diff>
--- a/resources/Pinbelegung.xlsx
+++ b/resources/Pinbelegung.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HofSpannung\Git\CarSoftware CAN Service\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HofSpannung\Git\CarSoftware CAN Service\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA37BD3-BEF8-4A94-809A-DD0381ECC59F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0CFF40-F9B2-4BAD-8E31-CE837B4BC461}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="23715" windowHeight="4950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="46">
   <si>
     <t>Dashboard</t>
   </si>
@@ -159,13 +159,22 @@
   </si>
   <si>
     <t>Signal Federweg hr</t>
+  </si>
+  <si>
+    <t>RPM Sensor vorne Links</t>
+  </si>
+  <si>
+    <t>RPM Sensor vorne Rechts</t>
+  </si>
+  <si>
+    <t>Ansteuerung über Relais</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,8 +196,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +231,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -245,25 +266,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -272,12 +293,18 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
     <cellStyle name="Neutral" xfId="2" builtinId="28"/>
+    <cellStyle name="Schlecht" xfId="3" builtinId="27"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -614,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:F31"/>
+  <dimension ref="C3:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,11 +655,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
@@ -655,7 +682,7 @@
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="D6" t="s">
@@ -663,7 +690,7 @@
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="4" t="s">
         <v>5</v>
       </c>
       <c r="D7" t="s">
@@ -671,40 +698,40 @@
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D8" t="s">
         <v>30</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="10" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="6"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D10" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
@@ -726,143 +753,156 @@
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="C16" s="12" t="s">
         <v>10</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="8" t="s">
+      <c r="E16" s="9" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="C17" s="12" t="s">
         <v>11</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="C18" s="12" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="9"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="10" t="s">
+      <c r="C19" s="5" t="s">
         <v>13</v>
       </c>
       <c r="D19" t="s">
         <v>23</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="9"/>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="10" t="s">
+      <c r="C20" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="E20" s="9"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="10" t="s">
+      <c r="C21" s="5" t="s">
         <v>15</v>
       </c>
       <c r="D21" t="s">
         <v>25</v>
       </c>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C24" s="7" t="s">
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-    </row>
-    <row r="25" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C25" s="1" t="s">
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C26" s="9" t="s">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D28" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E28" s="6" t="s">
         <v>35</v>
-      </c>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E27" s="6"/>
-    </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="29" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
+        <v>34</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" s="7"/>
+    </row>
+    <row r="30" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D30" t="s">
+        <v>39</v>
+      </c>
+      <c r="E30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
         <v>37</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D31" t="s">
         <v>30</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E31" s="11" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C32" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D32" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="3"/>
-    </row>
-    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D33" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E28:E29"/>
     <mergeCell ref="C13:E13"/>
     <mergeCell ref="C3:E3"/>
     <mergeCell ref="E16:E21"/>
     <mergeCell ref="E8:E10"/>
-    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C26:E26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update Brake Service (FSG Rules), Update Pins
</commit_message>
<xml_diff>
--- a/resources/Pinbelegung.xlsx
+++ b/resources/Pinbelegung.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HofSpannung\Git\CarSoftware CAN Service\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HofSpannung\Git\CarSoftware\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0CFF40-F9B2-4BAD-8E31-CE837B4BC461}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0B9B6F-F9B4-424A-B702-6EDFE992213A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="23715" windowHeight="4950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Dashboard</t>
   </si>
@@ -44,21 +44,6 @@
     <t>Erläuterung</t>
   </si>
   <si>
-    <t>Taster1</t>
-  </si>
-  <si>
-    <t>Taster2</t>
-  </si>
-  <si>
-    <t>LED1</t>
-  </si>
-  <si>
-    <t>LED2</t>
-  </si>
-  <si>
-    <t>LED3</t>
-  </si>
-  <si>
     <t>Pedalerie</t>
   </si>
   <si>
@@ -92,39 +77,9 @@
     <t>3,3V</t>
   </si>
   <si>
-    <t>A0</t>
-  </si>
-  <si>
-    <t>A1</t>
-  </si>
-  <si>
-    <t>A2</t>
-  </si>
-  <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
-  </si>
-  <si>
     <t>Zum Test können die Buchsenleisten auf dem Board benutzt werden. Als produktive Lösung nur die Pins.</t>
   </si>
   <si>
-    <t>D5</t>
-  </si>
-  <si>
-    <t>D3</t>
-  </si>
-  <si>
-    <t>D7</t>
-  </si>
-  <si>
-    <t>D6</t>
-  </si>
-  <si>
     <t>Für LEDs absichtlich PWM-fähige Pins verwendet</t>
   </si>
   <si>
@@ -146,12 +101,6 @@
     <t>Pumpe PWM</t>
   </si>
   <si>
-    <t>D9</t>
-  </si>
-  <si>
-    <t>D10</t>
-  </si>
-  <si>
     <t>Ansteuerung über Transistor</t>
   </si>
   <si>
@@ -168,6 +117,72 @@
   </si>
   <si>
     <t>Ansteuerung über Relais</t>
+  </si>
+  <si>
+    <t>PB_2 (rechts)</t>
+  </si>
+  <si>
+    <t>PB_4 (rechts)</t>
+  </si>
+  <si>
+    <t>PA_0 (links)</t>
+  </si>
+  <si>
+    <t>PB_0 (links)</t>
+  </si>
+  <si>
+    <t>PC_1 (links)</t>
+  </si>
+  <si>
+    <t>PB_1 (rechts)</t>
+  </si>
+  <si>
+    <t>PA_3 (rechts)</t>
+  </si>
+  <si>
+    <t>PC_4 (rechts)</t>
+  </si>
+  <si>
+    <t>Taster Start</t>
+  </si>
+  <si>
+    <t>Taster Reset</t>
+  </si>
+  <si>
+    <t>LED Grün</t>
+  </si>
+  <si>
+    <t>LED Gelb</t>
+  </si>
+  <si>
+    <t>LED Rot</t>
+  </si>
+  <si>
+    <t>PB_5 (rechts)</t>
+  </si>
+  <si>
+    <t>PA_10 (rechts)</t>
+  </si>
+  <si>
+    <t>PB_10 (rechts)</t>
+  </si>
+  <si>
+    <t>PC_7 (rechts)</t>
+  </si>
+  <si>
+    <t>PG_4 (rechts)</t>
+  </si>
+  <si>
+    <t>PE_13 (rechts)</t>
+  </si>
+  <si>
+    <t>PD_10 (rechts)</t>
+  </si>
+  <si>
+    <t>PE_10 (rechts)</t>
+  </si>
+  <si>
+    <t>PF_4 (rechts)</t>
   </si>
 </sst>
 </file>
@@ -281,6 +296,10 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -296,10 +315,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -643,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C3:F33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,11 +670,11 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
@@ -675,63 +690,63 @@
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" s="4" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>31</v>
+        <v>43</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="10"/>
+        <v>30</v>
+      </c>
+      <c r="E10" s="12"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
+      <c r="C13" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
@@ -746,84 +761,90 @@
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="12" t="s">
-        <v>10</v>
+      <c r="C16" s="7" t="s">
+        <v>5</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>26</v>
+        <v>34</v>
+      </c>
+      <c r="E16" s="11" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="12" t="s">
-        <v>11</v>
+      <c r="C17" s="7" t="s">
+        <v>6</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="9"/>
+        <v>31</v>
+      </c>
+      <c r="E17" s="11"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="12" t="s">
-        <v>12</v>
+      <c r="C18" s="7" t="s">
+        <v>7</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
-      </c>
-      <c r="E18" s="9"/>
+        <v>32</v>
+      </c>
+      <c r="E18" s="11"/>
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="9"/>
+        <v>33</v>
+      </c>
+      <c r="E19" s="11"/>
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C20" s="5" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="9"/>
+        <v>35</v>
+      </c>
+      <c r="E20" s="11"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C21" s="5" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D21" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="9"/>
+        <v>36</v>
+      </c>
+      <c r="E21" s="11"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
-        <v>43</v>
+        <v>26</v>
+      </c>
+      <c r="D22" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
-        <v>44</v>
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
+      <c r="C26" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
@@ -838,61 +859,61 @@
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C28" s="4" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E28" s="6" t="s">
-        <v>35</v>
+        <v>46</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="D29" t="s">
-        <v>29</v>
-      </c>
-      <c r="E29" s="7"/>
+        <v>47</v>
+      </c>
+      <c r="E29" s="9"/>
     </row>
     <row r="30" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="D30" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="3:5" ht="30" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="D31" t="s">
-        <v>30</v>
-      </c>
-      <c r="E31" s="11" t="s">
-        <v>40</v>
+        <v>49</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="12" t="s">
-        <v>41</v>
+      <c r="C32" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="D32" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="12" t="s">
-        <v>42</v>
+      <c r="C33" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="D33" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update README.md, Update Pins
</commit_message>
<xml_diff>
--- a/resources/Pinbelegung.xlsx
+++ b/resources/Pinbelegung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HofSpannung\Git\CarSoftware\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0B9B6F-F9B4-424A-B702-6EDFE992213A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33AC281-228D-4035-A6BD-43A6EE4E4F81}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="23715" windowHeight="4950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
   <si>
     <t>Dashboard</t>
   </si>
@@ -183,6 +183,15 @@
   </si>
   <si>
     <t>PF_4 (rechts)</t>
+  </si>
+  <si>
+    <t>RPM Sensor hinten Links</t>
+  </si>
+  <si>
+    <t>RPM Sensor hinten Rechts</t>
+  </si>
+  <si>
+    <t>PC_5 (rechts)</t>
   </si>
 </sst>
 </file>
@@ -656,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:F33"/>
+  <dimension ref="C3:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C18" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,6 +923,22 @@
       </c>
       <c r="D33" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C35" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add CoolingService, Bugfix, Update Pins
</commit_message>
<xml_diff>
--- a/resources/Pinbelegung.xlsx
+++ b/resources/Pinbelegung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HofSpannung\Git\CarSoftware\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95BCCB32-A852-475D-B0AC-2FE27C5EC70B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FAB6A9-8738-4F20-954C-E4C694CC4C02}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="23715" windowHeight="4950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Dashboard</t>
   </si>
@@ -192,6 +192,12 @@
   </si>
   <si>
     <t>PC_5 (rechts)</t>
+  </si>
+  <si>
+    <t>HV-Enabled Pin</t>
+  </si>
+  <si>
+    <t>PC_14 (links)</t>
   </si>
 </sst>
 </file>
@@ -665,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:F35"/>
+  <dimension ref="C3:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,7 +872,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="3:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="4" t="s">
         <v>18</v>
       </c>
@@ -939,6 +945,14 @@
       </c>
       <c r="D35" t="s">
         <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Pins for PCBs
</commit_message>
<xml_diff>
--- a/resources/Pinbelegung.xlsx
+++ b/resources/Pinbelegung.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HofSpannung\Git\CarSoftware\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\HofSpannung\Git\CarSoftware\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64FAB6A9-8738-4F20-954C-E4C694CC4C02}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D850A50C-7990-4C99-9327-85029BD4D50D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="150" windowWidth="23715" windowHeight="4950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="66">
   <si>
     <t>Dashboard</t>
   </si>
@@ -198,6 +198,36 @@
   </si>
   <si>
     <t>PC_14 (links)</t>
+  </si>
+  <si>
+    <t>Pinbezeichnung (PCB)</t>
+  </si>
+  <si>
+    <t>PA_1</t>
+  </si>
+  <si>
+    <t>PA_0</t>
+  </si>
+  <si>
+    <t>PA_14</t>
+  </si>
+  <si>
+    <t>PA_13</t>
+  </si>
+  <si>
+    <t>PA_15</t>
+  </si>
+  <si>
+    <t>PC_0</t>
+  </si>
+  <si>
+    <t>PC_1</t>
+  </si>
+  <si>
+    <t>PB_0</t>
+  </si>
+  <si>
+    <t>PA_4</t>
   </si>
 </sst>
 </file>
@@ -302,10 +332,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -674,7 +703,7 @@
   <dimension ref="C3:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,15 +711,16 @@
     <col min="3" max="3" width="44.140625" customWidth="1"/>
     <col min="4" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" customWidth="1"/>
+    <col min="6" max="6" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="2"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
     </row>
     <row r="4" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
@@ -700,6 +730,9 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -712,56 +745,72 @@
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>37</v>
       </c>
       <c r="D6" t="s">
         <v>45</v>
       </c>
+      <c r="E6" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D7" t="s">
         <v>44</v>
       </c>
+      <c r="E7" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>39</v>
       </c>
       <c r="D8" t="s">
         <v>43</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F8" s="11" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="3" t="s">
         <v>40</v>
       </c>
       <c r="D9" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="12"/>
+      <c r="E9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="11"/>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>41</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>
       </c>
-      <c r="E10" s="12"/>
+      <c r="E10" t="s">
+        <v>57</v>
+      </c>
+      <c r="F10" s="11"/>
     </row>
     <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C14" s="1" t="s">
@@ -771,6 +820,9 @@
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>3</v>
       </c>
     </row>
@@ -783,85 +835,110 @@
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D16" t="s">
         <v>34</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C17" s="7" t="s">
+    <row r="17" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C17" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D17" t="s">
         <v>35</v>
       </c>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C18" s="7" t="s">
+      <c r="E17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="10"/>
+    </row>
+    <row r="18" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C18" s="6" t="s">
         <v>7</v>
       </c>
       <c r="D18" t="s">
         <v>36</v>
       </c>
-      <c r="E18" s="11"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="5" t="s">
+      <c r="E18" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="10"/>
+    </row>
+    <row r="19" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C19" s="4" t="s">
         <v>8</v>
       </c>
       <c r="D19" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="11"/>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C20" s="5" t="s">
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="10"/>
+    </row>
+    <row r="20" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C21" s="5" t="s">
+      <c r="E20" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C21" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D21" t="s">
         <v>32</v>
       </c>
-      <c r="E21" s="11"/>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C22" s="4" t="s">
+      <c r="E21" t="s">
+        <v>62</v>
+      </c>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C22" s="3" t="s">
         <v>26</v>
       </c>
       <c r="D22" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C23" s="4" t="s">
+      <c r="E22" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C23" s="3" t="s">
         <v>27</v>
       </c>
       <c r="D23" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="26" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="10" t="s">
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="10"/>
-      <c r="E26" s="10"/>
-    </row>
-    <row r="27" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+    </row>
+    <row r="27" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C27" s="1" t="s">
         <v>1</v>
       </c>
@@ -869,62 +946,65 @@
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="4" t="s">
+    <row r="28" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C28" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D28" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="F28" s="7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C29" t="s">
         <v>19</v>
       </c>
       <c r="D29" t="s">
         <v>47</v>
       </c>
-      <c r="E29" s="9"/>
-    </row>
-    <row r="30" spans="3:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F29" s="8"/>
+    </row>
+    <row r="30" spans="3:6" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
         <v>21</v>
       </c>
       <c r="D30" t="s">
         <v>48</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="31" spans="3:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
         <v>22</v>
       </c>
       <c r="D31" t="s">
         <v>49</v>
       </c>
-      <c r="E31" s="6" t="s">
+      <c r="F31" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="C32" s="7" t="s">
+    <row r="32" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C32" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D32" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="3"/>
+      <c r="F32" s="2"/>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D33" t="s">
@@ -932,7 +1012,7 @@
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>51</v>
       </c>
       <c r="D34" t="s">
@@ -940,7 +1020,7 @@
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C35" s="4" t="s">
+      <c r="C35" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D35" t="s">
@@ -957,12 +1037,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="E16:E21"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="F16:F21"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>